<commit_message>
完成 - Node XLSX
</commit_message>
<xml_diff>
--- a/032-Node 工具库/src/common/language/dist/Excel 导出文件.xlsx
+++ b/032-Node 工具库/src/common/language/dist/Excel 导出文件.xlsx
@@ -379,17 +379,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>key</v>
+        <v>keys</v>
       </c>
       <c r="B1" t="str">
         <v>zh-CN</v>

</xml_diff>